<commit_message>
Update on comodoro.py and Pasta1.xlsx
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\Data science\Python\Projetos do Pirão\projeto_comodoro\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gráf1" sheetId="2" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="100">
   <si>
     <t>entregas</t>
   </si>
@@ -37,9 +42,6 @@
     <t>17:45 - 23:30</t>
   </si>
   <si>
-    <t>10:30 - 16:01</t>
-  </si>
-  <si>
     <t>confirmado</t>
   </si>
   <si>
@@ -49,15 +51,6 @@
     <t>18:00 - 00:00</t>
   </si>
   <si>
-    <t>18:00 - 00:01</t>
-  </si>
-  <si>
-    <t>18:00 - 00:03</t>
-  </si>
-  <si>
-    <t>18:00 - 00:05</t>
-  </si>
-  <si>
     <t>confrimado</t>
   </si>
   <si>
@@ -304,9 +297,6 @@
     <t>Pedro Gomes</t>
   </si>
   <si>
-    <t>Coxilha do Pampas</t>
-  </si>
-  <si>
     <t>Pizza NY</t>
   </si>
   <si>
@@ -332,9 +322,6 @@
   </si>
   <si>
     <t>Falaguata Bonfim</t>
-  </si>
-  <si>
-    <t>18:00 - 23:59</t>
   </si>
   <si>
     <t>Pizzaria 2 Irmãos - Loja 3</t>
@@ -928,151 +915,79 @@
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="41">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="43">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="44">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="46">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
@@ -4925,20 +4840,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41521920"/>
-        <c:axId val="41523456"/>
+        <c:axId val="-390741392"/>
+        <c:axId val="-390728880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41521920"/>
+        <c:axId val="-390741392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41523456"/>
+        <c:crossAx val="-390728880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4946,7 +4862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41523456"/>
+        <c:axId val="-390728880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4957,14 +4873,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41521920"/>
+        <c:crossAx val="-390741392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5267,7 +5182,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5277,8 +5192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5297,34 +5212,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5332,13 +5247,13 @@
         <v>45433</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -5364,13 +5279,10 @@
         <v>45433</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -5393,13 +5305,13 @@
         <v>45433</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -5425,13 +5337,10 @@
         <v>45433</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
@@ -5454,13 +5363,13 @@
         <v>45433</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -5486,13 +5395,10 @@
         <v>45433</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -5515,13 +5421,13 @@
         <v>45433</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -5547,13 +5453,10 @@
         <v>45433</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -5576,16 +5479,16 @@
         <v>45433</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
         <v>0</v>
@@ -5608,13 +5511,10 @@
         <v>45433</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
         <v>1</v>
@@ -5637,16 +5537,16 @@
         <v>45433</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>0</v>
@@ -5669,13 +5569,10 @@
         <v>45433</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>1</v>
@@ -5698,16 +5595,16 @@
         <v>45433</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
         <v>0</v>
@@ -5730,13 +5627,10 @@
         <v>45433</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
         <v>1</v>
@@ -5759,16 +5653,16 @@
         <v>45433</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
         <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -5791,13 +5685,10 @@
         <v>45433</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
         <v>1</v>
@@ -5820,16 +5711,16 @@
         <v>45433</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
         <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
       </c>
       <c r="F18" t="s">
         <v>0</v>
@@ -5852,13 +5743,10 @@
         <v>45433</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
         <v>1</v>
@@ -5881,13 +5769,13 @@
         <v>45433</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
@@ -5913,16 +5801,16 @@
         <v>45433</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
         <v>0</v>
@@ -5945,13 +5833,10 @@
         <v>45433</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
         <v>1</v>
@@ -5974,16 +5859,16 @@
         <v>45433</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
         <v>0</v>
@@ -6006,16 +5891,16 @@
         <v>45433</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
         <v>0</v>
@@ -6038,13 +5923,10 @@
         <v>45433</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
         <v>1</v>
@@ -6067,16 +5949,16 @@
         <v>45433</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
         <v>0</v>
@@ -6099,13 +5981,10 @@
         <v>45433</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
         <v>1</v>
@@ -6128,16 +6007,16 @@
         <v>45433</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F28" t="s">
         <v>0</v>
@@ -6160,13 +6039,10 @@
         <v>45433</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
         <v>1</v>
@@ -6189,16 +6065,16 @@
         <v>45433</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
         <v>0</v>
@@ -6221,13 +6097,10 @@
         <v>45433</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
         <v>1</v>
@@ -6250,16 +6123,16 @@
         <v>45433</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F32" t="s">
         <v>0</v>
@@ -6282,13 +6155,10 @@
         <v>45433</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
         <v>1</v>
@@ -6311,13 +6181,13 @@
         <v>45433</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
@@ -6343,13 +6213,10 @@
         <v>45433</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F35" t="s">
         <v>1</v>
@@ -6372,13 +6239,13 @@
         <v>45433</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
         <v>3</v>
@@ -6404,13 +6271,10 @@
         <v>45433</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F37" t="s">
         <v>1</v>
@@ -6433,16 +6297,16 @@
         <v>45433</v>
       </c>
       <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
         <v>35</v>
       </c>
-      <c r="C38" t="s">
-        <v>39</v>
-      </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F38" t="s">
         <v>0</v>
@@ -6465,13 +6329,10 @@
         <v>45433</v>
       </c>
       <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
         <v>35</v>
-      </c>
-      <c r="C39" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
       </c>
       <c r="F39" t="s">
         <v>1</v>
@@ -6494,16 +6355,16 @@
         <v>45433</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F40" t="s">
         <v>0</v>
@@ -6526,13 +6387,10 @@
         <v>45433</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F41" t="s">
         <v>1</v>
@@ -6555,16 +6413,16 @@
         <v>45433</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F42" t="s">
         <v>0</v>
@@ -6587,13 +6445,10 @@
         <v>45433</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F43" t="s">
         <v>1</v>
@@ -6616,16 +6471,16 @@
         <v>45433</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F44" t="s">
         <v>0</v>
@@ -6648,13 +6503,10 @@
         <v>45433</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F45" t="s">
         <v>1</v>
@@ -6677,16 +6529,16 @@
         <v>45433</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F46" t="s">
         <v>0</v>
@@ -6709,13 +6561,10 @@
         <v>45433</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="F47" t="s">
         <v>1</v>
@@ -6738,16 +6587,16 @@
         <v>45433</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F48" t="s">
         <v>0</v>
@@ -6770,13 +6619,10 @@
         <v>45433</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F49" t="s">
         <v>1</v>
@@ -6799,16 +6645,16 @@
         <v>45433</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F50" t="s">
         <v>0</v>
@@ -6831,13 +6677,10 @@
         <v>45433</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="F51" t="s">
         <v>1</v>
@@ -6860,16 +6703,16 @@
         <v>45433</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F52" t="s">
         <v>0</v>
@@ -6892,13 +6735,10 @@
         <v>45433</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F53" t="s">
         <v>1</v>
@@ -6921,16 +6761,16 @@
         <v>45433</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F54" t="s">
         <v>0</v>
@@ -6953,13 +6793,10 @@
         <v>45433</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="F55" t="s">
         <v>1</v>
@@ -6982,16 +6819,16 @@
         <v>45433</v>
       </c>
       <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" t="s">
         <v>60</v>
       </c>
-      <c r="C56" t="s">
-        <v>64</v>
-      </c>
       <c r="D56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E56" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F56" t="s">
         <v>0</v>
@@ -7014,13 +6851,10 @@
         <v>45433</v>
       </c>
       <c r="B57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" t="s">
         <v>60</v>
-      </c>
-      <c r="C57" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
       </c>
       <c r="F57" t="s">
         <v>1</v>
@@ -7043,16 +6877,16 @@
         <v>45433</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F58" t="s">
         <v>0</v>
@@ -7075,13 +6909,10 @@
         <v>45433</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="F59" t="s">
         <v>1</v>
@@ -7104,16 +6935,16 @@
         <v>45433</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F60" t="s">
         <v>0</v>
@@ -7136,13 +6967,10 @@
         <v>45433</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F61" t="s">
         <v>1</v>
@@ -7165,16 +6993,16 @@
         <v>45433</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F62" t="s">
         <v>0</v>
@@ -7197,13 +7025,10 @@
         <v>45433</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="F63" t="s">
         <v>1</v>
@@ -7226,16 +7051,16 @@
         <v>45433</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C64" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F64" t="s">
         <v>0</v>
@@ -7258,13 +7083,10 @@
         <v>45433</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>71</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="F65" t="s">
         <v>1</v>
@@ -7287,16 +7109,16 @@
         <v>45433</v>
       </c>
       <c r="B66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" t="s">
         <v>68</v>
       </c>
-      <c r="C66" t="s">
-        <v>72</v>
-      </c>
       <c r="D66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F66" t="s">
         <v>0</v>
@@ -7319,13 +7141,10 @@
         <v>45433</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>73</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F67" t="s">
         <v>1</v>
@@ -7348,16 +7167,16 @@
         <v>45433</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="s">
         <v>0</v>
@@ -7380,16 +7199,16 @@
         <v>45433</v>
       </c>
       <c r="B69" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="s">
         <v>0</v>
@@ -7412,16 +7231,16 @@
         <v>45433</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E70" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F70" t="s">
         <v>0</v>
@@ -7444,16 +7263,16 @@
         <v>45433</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F71" t="s">
         <v>0</v>
@@ -7476,16 +7295,16 @@
         <v>45433</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F72" t="s">
         <v>0</v>
@@ -7508,16 +7327,16 @@
         <v>45433</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C73" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" t="s">
         <v>83</v>
-      </c>
-      <c r="D73" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" t="s">
-        <v>87</v>
       </c>
       <c r="F73" t="s">
         <v>0</v>
@@ -7540,13 +7359,10 @@
         <v>45433</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C74" t="s">
-        <v>83</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="F74" t="s">
         <v>1</v>
@@ -7569,16 +7385,16 @@
         <v>45433</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E75" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F75" t="s">
         <v>0</v>
@@ -7601,13 +7417,10 @@
         <v>45433</v>
       </c>
       <c r="B76" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>84</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F76" t="s">
         <v>1</v>
@@ -7630,16 +7443,16 @@
         <v>45433</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C77" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E77" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="s">
         <v>0</v>
@@ -7662,16 +7475,16 @@
         <v>45433</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C78" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="s">
         <v>0</v>
@@ -7694,13 +7507,13 @@
         <v>45432</v>
       </c>
       <c r="B79" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C79" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E79" t="s">
         <v>2</v>
@@ -7726,13 +7539,10 @@
         <v>45432</v>
       </c>
       <c r="B80" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C80" t="s">
-        <v>28</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F80" t="s">
         <v>1</v>
@@ -7755,13 +7565,13 @@
         <v>45432</v>
       </c>
       <c r="B81" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E81" t="s">
         <v>2</v>
@@ -7787,13 +7597,10 @@
         <v>45432</v>
       </c>
       <c r="B82" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F82" t="s">
         <v>1</v>
@@ -7816,13 +7623,13 @@
         <v>45432</v>
       </c>
       <c r="B83" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E83" t="s">
         <v>2</v>
@@ -7848,13 +7655,10 @@
         <v>45432</v>
       </c>
       <c r="B84" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C84" t="s">
-        <v>21</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F84" t="s">
         <v>1</v>
@@ -7877,16 +7681,16 @@
         <v>45432</v>
       </c>
       <c r="B85" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C85" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F85" t="s">
         <v>0</v>
@@ -7909,13 +7713,10 @@
         <v>45432</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C86" t="s">
-        <v>91</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="F86" t="s">
         <v>1</v>
@@ -7938,16 +7739,16 @@
         <v>45432</v>
       </c>
       <c r="B87" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F87" t="s">
         <v>0</v>
@@ -7970,13 +7771,10 @@
         <v>45432</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C88" t="s">
-        <v>92</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="F88" t="s">
         <v>1</v>
@@ -7999,16 +7797,16 @@
         <v>45432</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C89" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E89" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F89" t="s">
         <v>0</v>
@@ -8031,13 +7829,10 @@
         <v>45432</v>
       </c>
       <c r="B90" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F90" t="s">
         <v>1</v>
@@ -8060,16 +7855,16 @@
         <v>45432</v>
       </c>
       <c r="B91" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C91" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F91" t="s">
         <v>0</v>
@@ -8092,13 +7887,10 @@
         <v>45432</v>
       </c>
       <c r="B92" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C92" t="s">
-        <v>14</v>
-      </c>
-      <c r="D92">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F92" t="s">
         <v>1</v>
@@ -8121,16 +7913,16 @@
         <v>45432</v>
       </c>
       <c r="B93" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C93" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E93" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F93" t="s">
         <v>0</v>
@@ -8153,13 +7945,10 @@
         <v>45432</v>
       </c>
       <c r="B94" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C94" t="s">
-        <v>36</v>
-      </c>
-      <c r="D94">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F94" t="s">
         <v>1</v>
@@ -8182,16 +7971,16 @@
         <v>45432</v>
       </c>
       <c r="B95" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C95" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D95" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E95" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F95" t="s">
         <v>0</v>
@@ -8214,13 +8003,10 @@
         <v>45432</v>
       </c>
       <c r="B96" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C96" t="s">
-        <v>71</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="F96" t="s">
         <v>1</v>
@@ -8243,16 +8029,16 @@
         <v>45432</v>
       </c>
       <c r="B97" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C97" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D97" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E97" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F97" t="s">
         <v>0</v>
@@ -8275,13 +8061,10 @@
         <v>45432</v>
       </c>
       <c r="B98" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C98" t="s">
-        <v>93</v>
-      </c>
-      <c r="D98">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="F98" t="s">
         <v>1</v>
@@ -8304,16 +8087,16 @@
         <v>45432</v>
       </c>
       <c r="B99" t="s">
+        <v>64</v>
+      </c>
+      <c r="C99" t="s">
         <v>68</v>
       </c>
-      <c r="C99" t="s">
-        <v>72</v>
-      </c>
       <c r="D99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E99" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F99" t="s">
         <v>0</v>
@@ -8336,13 +8119,10 @@
         <v>45432</v>
       </c>
       <c r="B100" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" t="s">
         <v>68</v>
-      </c>
-      <c r="C100" t="s">
-        <v>72</v>
-      </c>
-      <c r="D100">
-        <v>0</v>
       </c>
       <c r="F100" t="s">
         <v>1</v>
@@ -8365,13 +8145,13 @@
         <v>45432</v>
       </c>
       <c r="B101" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D101" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E101" t="s">
         <v>3</v>
@@ -8397,13 +8177,10 @@
         <v>45432</v>
       </c>
       <c r="B102" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>26</v>
-      </c>
-      <c r="D102">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F102" t="s">
         <v>1</v>
@@ -8426,13 +8203,13 @@
         <v>45432</v>
       </c>
       <c r="B103" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E103" t="s">
         <v>3</v>
@@ -8458,13 +8235,10 @@
         <v>45432</v>
       </c>
       <c r="B104" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>84</v>
-      </c>
-      <c r="D104">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F104" t="s">
         <v>1</v>
@@ -8487,16 +8261,16 @@
         <v>45432</v>
       </c>
       <c r="B105" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="C105" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E105" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F105" t="s">
         <v>0</v>
@@ -8519,13 +8293,10 @@
         <v>45432</v>
       </c>
       <c r="B106" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>39</v>
-      </c>
-      <c r="D106">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F106" t="s">
         <v>1</v>
@@ -8548,16 +8319,16 @@
         <v>45432</v>
       </c>
       <c r="B107" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C107" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D107" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E107" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F107" t="s">
         <v>0</v>
@@ -8580,13 +8351,10 @@
         <v>45432</v>
       </c>
       <c r="B108" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C108" t="s">
-        <v>47</v>
-      </c>
-      <c r="D108">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F108" t="s">
         <v>1</v>
@@ -8609,16 +8377,16 @@
         <v>45432</v>
       </c>
       <c r="B109" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C109" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F109" t="s">
         <v>0</v>
@@ -8641,16 +8409,16 @@
         <v>45432</v>
       </c>
       <c r="B110" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C110" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D110" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E110" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F110" t="s">
         <v>0</v>
@@ -8673,13 +8441,10 @@
         <v>45432</v>
       </c>
       <c r="B111" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C111" t="s">
-        <v>66</v>
-      </c>
-      <c r="D111">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="F111" t="s">
         <v>1</v>
@@ -8702,13 +8467,13 @@
         <v>45432</v>
       </c>
       <c r="B112" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C112" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D112" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E112" t="s">
         <v>4</v>
@@ -8734,16 +8499,16 @@
         <v>45432</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C113" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D113" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E113" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F113" t="s">
         <v>0</v>
@@ -8766,16 +8531,16 @@
         <v>45432</v>
       </c>
       <c r="B114" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C114" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D114" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E114" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F114" t="s">
         <v>0</v>
@@ -8798,13 +8563,10 @@
         <v>45432</v>
       </c>
       <c r="B115" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C115" t="s">
-        <v>81</v>
-      </c>
-      <c r="D115">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F115" t="s">
         <v>1</v>
@@ -8827,16 +8589,16 @@
         <v>45432</v>
       </c>
       <c r="B116" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C116" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D116" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E116" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F116" t="s">
         <v>0</v>
@@ -8859,16 +8621,16 @@
         <v>45432</v>
       </c>
       <c r="B117" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C117" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D117" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E117" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F117" t="s">
         <v>0</v>
@@ -8891,13 +8653,10 @@
         <v>45432</v>
       </c>
       <c r="B118" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C118" t="s">
-        <v>78</v>
-      </c>
-      <c r="D118">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="F118" t="s">
         <v>1</v>
@@ -8920,16 +8679,16 @@
         <v>45432</v>
       </c>
       <c r="B119" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C119" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E119" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F119" t="s">
         <v>0</v>
@@ -8952,16 +8711,16 @@
         <v>45432</v>
       </c>
       <c r="B120" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C120" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D120" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E120" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F120" t="s">
         <v>0</v>
@@ -8984,16 +8743,16 @@
         <v>45432</v>
       </c>
       <c r="B121" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C121" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D121" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E121" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="F121" t="s">
         <v>0</v>
@@ -9016,13 +8775,10 @@
         <v>45432</v>
       </c>
       <c r="B122" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C122" t="s">
-        <v>62</v>
-      </c>
-      <c r="D122">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F122" t="s">
         <v>1</v>

</xml_diff>